<commit_message>
mehnoor and mahrosh left
</commit_message>
<xml_diff>
--- a/mid term spreadsheet.xlsx
+++ b/mid term spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kma\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kma\Desktop\ahmed-html-work\kma-learning - test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0EC9CDD-BB04-4959-B831-87E3186DA263}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C20289-5F69-4C69-A6C8-702118191FA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -443,7 +443,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -465,7 +465,7 @@
       <c r="H1" s="4"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -494,7 +494,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>10</v>
       </c>
@@ -525,25 +525,33 @@
         <v>#NAME?</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
+      <c r="C4" s="2">
+        <v>9</v>
+      </c>
+      <c r="D4" s="2">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2">
+        <v>10</v>
+      </c>
       <c r="G4" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="H4" s="2">
         <v>50</v>
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>12</v>
       </c>
@@ -569,7 +577,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
@@ -595,7 +603,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
@@ -621,25 +629,33 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
+      <c r="C8" s="2">
+        <v>9</v>
+      </c>
+      <c r="D8" s="2">
+        <v>8</v>
+      </c>
+      <c r="E8" s="2">
+        <v>9</v>
+      </c>
+      <c r="F8" s="2">
+        <v>10</v>
+      </c>
       <c r="G8" s="2">
-        <f t="shared" si="0"/>
-        <v>0</v>
+        <f>SUM(B8:F8)</f>
+        <v>36</v>
       </c>
       <c r="H8" s="2">
         <v>50</v>
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>16</v>
       </c>
@@ -665,7 +681,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>17</v>
       </c>
@@ -691,7 +707,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -717,25 +733,33 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="2">
+        <v>8</v>
+      </c>
+      <c r="D12" s="2">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10</v>
+      </c>
       <c r="G12" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="H12" s="2">
         <v>50</v>
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>20</v>
       </c>
@@ -753,25 +777,33 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="C14" s="2">
+        <v>5</v>
+      </c>
+      <c r="D14" s="2">
+        <v>4</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1</v>
+      </c>
+      <c r="F14" s="2">
+        <v>10</v>
+      </c>
       <c r="G14" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="H14" s="2">
         <v>50</v>
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>22</v>
       </c>
@@ -789,7 +821,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
@@ -807,7 +839,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:9" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>

</xml_diff>